<commit_message>
Added motor controller and batteries to the BOM
</commit_message>
<xml_diff>
--- a/Mechanical/BOMs/Chassis BOM.xlsx
+++ b/Mechanical/BOMs/Chassis BOM.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="10380" windowHeight="9090"/>
+    <workbookView xWindow="360" yWindow="40" windowWidth="22460" windowHeight="14260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="114210"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Item</t>
   </si>
@@ -102,15 +107,6 @@
     <t>Zinc-Plated Steel Flat Head Socket Cap Screw (10-32, 1" Long) Pack of 25</t>
   </si>
   <si>
-    <t>Battery</t>
-  </si>
-  <si>
-    <t>Battery Charger</t>
-  </si>
-  <si>
-    <t>Motor Controller</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
@@ -124,15 +120,40 @@
   </si>
   <si>
     <t>http://www.trossenrobotics.com/store/p/5719-Pololu-Ball-Caster-with-1-2-Plastic-Ball.aspx</t>
+  </si>
+  <si>
+    <t>TE-088-210</t>
+  </si>
+  <si>
+    <t>Superdroid Robotics</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.superdroidrobots.com/shop/item.asp?itemid=793</t>
+  </si>
+  <si>
+    <t>12V 2200 mAHr NiMH 2x5 Battery Pack w/ Connectors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.superdroidrobots.com/shop/item.asp?itemid=821&amp;catid=5</t>
+  </si>
+  <si>
+    <t>Superdroid Robotics</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sabertooth Dual 10A Motor Driver</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TE-091-210</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
   <fonts count="10">
     <font>
       <sz val="10"/>
@@ -177,7 +198,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -192,18 +212,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -598,7 +612,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -660,27 +674,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -690,25 +683,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -720,31 +710,22 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -764,6 +745,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -771,7 +788,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -1059,75 +1076,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="0.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="46.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="0.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="6" width="10.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="79" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:9" ht="18" thickBot="1">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="36"/>
-    </row>
-    <row r="2" spans="1:9" ht="13.5" thickBot="1">
-      <c r="A2" s="48" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" spans="1:9" ht="13" thickBot="1">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="37" t="s">
-        <v>31</v>
+      <c r="I2" s="29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="26">
         <v>1</v>
       </c>
       <c r="E3" s="1">
@@ -1137,22 +1155,22 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G13" si="0">D3*E3</f>
+        <f t="shared" ref="G3:G12" si="0">D3*E3</f>
         <v>6.78</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="29" t="s">
-        <v>32</v>
+      <c r="I3" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="31.5" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="38" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="30" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="3">
@@ -1171,15 +1189,15 @@
       <c r="H4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="29" t="s">
-        <v>32</v>
+      <c r="I4" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1199,8 +1217,8 @@
       <c r="H5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>32</v>
+      <c r="I5" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="27" customHeight="1">
@@ -1227,15 +1245,15 @@
       <c r="H6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="39" t="s">
-        <v>34</v>
+      <c r="I6" s="31" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="20" t="s">
         <v>17</v>
       </c>
@@ -1255,8 +1273,8 @@
       <c r="H7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="28" t="s">
-        <v>33</v>
+      <c r="I7" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1">
@@ -1283,7 +1301,7 @@
       <c r="H8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="28"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1">
       <c r="A9" s="15" t="s">
@@ -1309,89 +1327,114 @@
       <c r="H9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="56" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A10" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="51">
+        <v>2</v>
+      </c>
+      <c r="E10" s="52">
+        <v>26.95</v>
+      </c>
+      <c r="F10" s="52"/>
+      <c r="G10" s="53">
+        <f t="shared" si="0"/>
+        <v>53.9</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="55" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A10" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="31"/>
-    </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A11" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="31"/>
-    </row>
-    <row r="12" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A12" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="31"/>
-    </row>
-    <row r="13" spans="1:9" ht="13.5" thickBot="1">
-      <c r="A13" s="54" t="s">
+    <row r="11" spans="1:9" s="56" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A11" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="51">
+        <v>1</v>
+      </c>
+      <c r="E11" s="52">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53">
+        <f t="shared" si="0"/>
+        <v>79.989999999999995</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="13" thickBot="1">
+      <c r="A12" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="5" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E12" s="6">
         <v>29.44</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F12" s="6">
         <v>0</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G12" s="32">
         <f t="shared" si="0"/>
         <v>29.44</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="30" t="s">
-        <v>32</v>
-      </c>
+      <c r="I12" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="10"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -1400,43 +1443,43 @@
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="A16" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="46">
+        <f>SUM(G3:G12)</f>
+        <v>317.2</v>
+      </c>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="43">
-        <f>SUM(G3:G13)</f>
-        <v>183.31</v>
-      </c>
+      <c r="G17" s="47"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="44"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1445,8 +1488,8 @@
       <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1455,8 +1498,8 @@
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="42"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -1465,8 +1508,8 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="42"/>
-      <c r="B22" s="42"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1475,8 +1518,8 @@
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="42"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1485,8 +1528,8 @@
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="42"/>
-      <c r="B24" s="42"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1495,8 +1538,8 @@
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="42"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1505,8 +1548,8 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1515,8 +1558,8 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="42"/>
-      <c r="B27" s="42"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1525,8 +1568,8 @@
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -1535,8 +1578,8 @@
       <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="42"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -1545,8 +1588,8 @@
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="42"/>
-      <c r="B30" s="42"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -1554,80 +1597,87 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-    </row>
+    <row r="31" spans="1:8" ht="21"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A17:E18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1"/>
     <hyperlink ref="I4" r:id="rId2"/>
     <hyperlink ref="I5" r:id="rId3"/>
-    <hyperlink ref="I13" r:id="rId4"/>
+    <hyperlink ref="I12" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>